<commit_message>
feat(lab): NIT/DPI + geo GT (22 deptos/338 munis); extracción depto/muni; UI fade; listado rápido; seed/reset
</commit_message>
<xml_diff>
--- a/db_docs/Listados/listado_tablas.xlsx
+++ b/db_docs/Listados/listado_tablas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,7 +484,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -502,24 +502,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>nextval('planes_id_seq'::regclass)</t>
+          <t>nextval('national_id_rules_id_seq'::regclass)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>country_id</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VARCHAR(100)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D4" t="b">
@@ -530,38 +530,38 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>id_type</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>VARCHAR(20)</t>
         </is>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>max_notarios</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(80)</t>
         </is>
       </c>
       <c r="D6" t="b">
@@ -572,33 +572,33 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>max_procuradores</t>
+          <t>regex</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(200)</t>
         </is>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>max_asistentes</t>
+          <t>dept_from_end</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -607,19 +607,19 @@
         </is>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>max_documentos</t>
+          <t>dept_len</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -628,19 +628,19 @@
         </is>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>storage_mb</t>
+          <t>muni_from_end</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -649,45 +649,45 @@
         </is>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>precio_mensual</t>
+          <t>muni_len</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DOUBLE PRECISION</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>national_id_rules</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>es_personalizado</t>
+          <t>notes</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>TEXT</t>
         </is>
       </c>
       <c r="D12" t="b">
@@ -698,105 +698,105 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>geo_admin2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>activo</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nextval('geo_admin2_id_seq'::regclass)</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>geo_admin2</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>fecha_creacion</t>
+          <t>country_id</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TIMESTAMP</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>planes</t>
+          <t>geo_admin2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>fecha_actualizacion</t>
+          <t>admin1_id</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TIMESTAMP</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>geo_admin2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>code</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(10)</t>
         </is>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nextval('bufetes_juridicos_id_seq'::regclass)</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>geo_admin2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>nombre_bufete_o_razon_social</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>VARCHAR(120)</t>
         </is>
       </c>
       <c r="D17" t="b">
@@ -807,17 +807,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>geo_admin2</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>direccion</t>
+          <t>type_name</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>VARCHAR(40)</t>
         </is>
       </c>
       <c r="D18" t="b">
@@ -828,59 +828,63 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>telefono</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>VARCHAR(50)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>nextval('planes_id_seq'::regclass)</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>VARCHAR(150)</t>
+          <t>VARCHAR(100)</t>
         </is>
       </c>
       <c r="D20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>nit</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>VARCHAR(50)</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D21" t="b">
@@ -891,80 +895,80 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>pais</t>
+          <t>max_notarios</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>VARCHAR(50)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>app_copyright</t>
+          <t>max_procuradores</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>nombre_aplicacion</t>
+          <t>max_asistentes</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>maneja_inventario_timbres_papel</t>
+          <t>max_documentos</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D25" t="b">
@@ -975,17 +979,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>incluye_libreria_plantillas_inicial</t>
+          <t>storage_mb</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D26" t="b">
@@ -996,17 +1000,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>habilita_auditoria_borrado_logico</t>
+          <t>precio_mensual</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>DOUBLE PRECISION</t>
         </is>
       </c>
       <c r="D27" t="b">
@@ -1017,12 +1021,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>habilita_dashboard_avanzado</t>
+          <t>es_personalizado</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1031,19 +1035,19 @@
         </is>
       </c>
       <c r="D28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>habilita_ayuda_contextual</t>
+          <t>activo</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1052,24 +1056,24 @@
         </is>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>facturacion_nombre</t>
+          <t>fecha_creacion</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>TIMESTAMP</t>
         </is>
       </c>
       <c r="D30" t="b">
@@ -1080,17 +1084,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>bufetes_juridicos</t>
+          <t>planes</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>facturacion_nit</t>
+          <t>fecha_actualizacion</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>VARCHAR(50)</t>
+          <t>TIMESTAMP</t>
         </is>
       </c>
       <c r="D31" t="b">
@@ -1106,18 +1110,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>facturacion_direccion</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>nextval('bufetes_juridicos_id_seq'::regclass)</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1127,16 +1135,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>formas_pago</t>
+          <t>nombre_bufete</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>VARCHAR(150)</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr"/>
     </row>
@@ -1148,12 +1156,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>metodo_pago_preferido</t>
+          <t>direccion</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>VARCHAR(50)</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D34" t="b">
@@ -1169,12 +1177,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>activo</t>
+          <t>telefono</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>VARCHAR(50)</t>
         </is>
       </c>
       <c r="D35" t="b">
@@ -1190,12 +1198,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>fecha_creacion</t>
+          <t>email</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TIMESTAMP</t>
+          <t>VARCHAR(150)</t>
         </is>
       </c>
       <c r="D36" t="b">
@@ -1211,12 +1219,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>plan_id</t>
+          <t>nit</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(50)</t>
         </is>
       </c>
       <c r="D37" t="b">
@@ -1227,84 +1235,80 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>cuenta_corriente</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>pais</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(50)</t>
         </is>
       </c>
       <c r="D38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>nextval('cuenta_corriente_id_seq'::regclass)</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>cuenta_corriente</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>bufete_id</t>
+          <t>maneja_inventario_timbres_papel</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>cuenta_corriente</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>incluye_libreria_plantillas_inicial</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>cuenta_corriente</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>habilita_auditoria_borrado_logico</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>VARCHAR(200)</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D41" t="b">
@@ -1315,17 +1319,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>cuenta_corriente</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>monto</t>
+          <t>habilita_dashboard_avanzado</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>DOUBLE PRECISION</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D42" t="b">
@@ -1336,84 +1340,80 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>pagos_bufete</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>habilita_ayuda_contextual</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>nextval('pagos_bufete_id_seq'::regclass)</t>
-        </is>
-      </c>
+      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>pagos_bufete</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>bufete_id</t>
+          <t>habilita_papeleria_digital</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>pagos_bufete</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>monto_pagado</t>
+          <t>forma_contacto</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>DOUBLE PRECISION</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>pagos_bufete</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>fecha_pago</t>
+          <t>facturacion_nombre</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D46" t="b">
@@ -1424,38 +1424,38 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>pagos_bufete</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>forma_pago</t>
+          <t>facturacion_nit</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>VARCHAR(8)</t>
+          <t>VARCHAR(50)</t>
         </is>
       </c>
       <c r="D47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>pagos_bufete</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>detalle</t>
+          <t>facturacion_direccion</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>VARCHAR(250)</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D48" t="b">
@@ -1466,63 +1466,59 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>formas_pago</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(150)</t>
         </is>
       </c>
       <c r="D49" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>nextval('usuarios_id_seq'::regclass)</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>username</t>
+          <t>metodo_pago_preferido</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>VARCHAR(150)</t>
+          <t>VARCHAR(50)</t>
         </is>
       </c>
       <c r="D50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>correo</t>
+          <t>activo</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>VARCHAR(150)</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D51" t="b">
@@ -1533,80 +1529,84 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>password_hash</t>
+          <t>fecha_creacion</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>TIMESTAMP</t>
         </is>
       </c>
       <c r="D52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>bufetes_juridicos</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>rol</t>
+          <t>plan_id</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>VARCHAR(13)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>cuenta_corriente</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>estado</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>VARCHAR(10)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D54" t="b">
-        <v>1</v>
-      </c>
-      <c r="E54" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>nextval('cuenta_corriente_id_seq'::regclass)</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>cuenta_corriente</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>nombres</t>
+          <t>bufete_id</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>VARCHAR(100)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D55" t="b">
@@ -1617,17 +1617,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>cuenta_corriente</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>apellidos</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>VARCHAR(100)</t>
+          <t>DATE</t>
         </is>
       </c>
       <c r="D56" t="b">
@@ -1638,70 +1638,74 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>cuenta_corriente</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>telefono</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>VARCHAR(20)</t>
+          <t>VARCHAR(200)</t>
         </is>
       </c>
       <c r="D57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>cuenta_corriente</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>direccion_laboral</t>
+          <t>monto</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>DOUBLE PRECISION</t>
         </is>
       </c>
       <c r="D58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>pagos_bufete</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>preferencia_contacto_red_social</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>VARCHAR(100)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D59" t="b">
-        <v>1</v>
-      </c>
-      <c r="E59" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>nextval('pagos_bufete_id_seq'::regclass)</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>pagos_bufete</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1722,100 +1726,96 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>usuarios</t>
+          <t>pagos_bufete</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>borrado_logico</t>
+          <t>monto_pagado</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>DOUBLE PRECISION</t>
         </is>
       </c>
       <c r="D61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>asistentes</t>
+          <t>pagos_bufete</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>fecha_pago</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>DATE</t>
         </is>
       </c>
       <c r="D62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>notario_procurador_asociacion</t>
+          <t>pagos_bufete</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>forma_pago</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(8)</t>
         </is>
       </c>
       <c r="D63" t="b">
         <v>0</v>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>nextval('notario_procurador_asociacion_id_seq'::regclass)</t>
-        </is>
-      </c>
+      <c r="E63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>notario_procurador_asociacion</t>
+          <t>pagos_bufete</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>notario_id</t>
+          <t>detalle</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(250)</t>
         </is>
       </c>
       <c r="D64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>notario_procurador_asociacion</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>procurador_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1826,22 +1826,26 @@
       <c r="D65" t="b">
         <v>0</v>
       </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>nextval('usuarios_id_seq'::regclass)</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>notario_procurador_asociacion</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>bufete_id</t>
+          <t>username</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(150)</t>
         </is>
       </c>
       <c r="D66" t="b">
@@ -1852,17 +1856,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>notario_procurador_asociacion</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>fecha_asignacion</t>
+          <t>correo</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>TIMESTAMP</t>
+          <t>VARCHAR(150)</t>
         </is>
       </c>
       <c r="D67" t="b">
@@ -1873,59 +1877,59 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>notario_procurador_asociacion</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>fecha_reasignacion</t>
+          <t>password_hash</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>TIMESTAMP</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>notario_procurador_asociacion</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>motivo_reasignacion</t>
+          <t>rol</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>VARCHAR(255)</t>
+          <t>VARCHAR(13)</t>
         </is>
       </c>
       <c r="D69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>notario_procurador_asociacion</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>activo</t>
+          <t>estado</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>VARCHAR(10)</t>
         </is>
       </c>
       <c r="D70" t="b">
@@ -1936,80 +1940,80 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>notarios</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>nombres</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(100)</t>
         </is>
       </c>
       <c r="D71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>notarios</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>numero_colegiado</t>
+          <t>apellidos</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>VARCHAR(20)</t>
+          <t>VARCHAR(100)</t>
         </is>
       </c>
       <c r="D72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>notarios</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>colegiado_activo</t>
+          <t>telefono</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>VARCHAR(20)</t>
         </is>
       </c>
       <c r="D73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>notarios</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>fecha_verificacion</t>
+          <t>direccion_laboral</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>TIMESTAMP</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D74" t="b">
@@ -2020,17 +2024,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>notarios</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>firma_electronica_registrada</t>
+          <t>preferencia_contacto_red_social</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>VARCHAR(100)</t>
         </is>
       </c>
       <c r="D75" t="b">
@@ -2041,17 +2045,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>notarios</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>proveedor_firma_electronica</t>
+          <t>bufete_id</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>VARCHAR(100)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D76" t="b">
@@ -2062,28 +2066,28 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>procuradores</t>
+          <t>usuarios</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>borrado_logico</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>asistentes</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2099,42 +2103,42 @@
       <c r="D78" t="b">
         <v>0</v>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>nextval('documentos_notariales_id_seq'::regclass)</t>
-        </is>
-      </c>
+      <c r="E78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notario_procurador_asociacion</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>tipo_documento</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>VARCHAR(17)</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D79" t="b">
         <v>0</v>
       </c>
-      <c r="E79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>nextval('notario_procurador_asociacion_id_seq'::regclass)</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notario_procurador_asociacion</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>numero_instrumento</t>
+          <t>notario_id</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2150,17 +2154,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notario_procurador_asociacion</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>fecha_otorgamiento</t>
+          <t>procurador_id</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D81" t="b">
@@ -2171,38 +2175,38 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notario_procurador_asociacion</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>hora_otorgamiento</t>
+          <t>bufete_id</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>TIME</t>
+          <t>INTEGER</t>
         </is>
       </c>
       <c r="D82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notario_procurador_asociacion</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>lugar_otorgamiento</t>
+          <t>fecha_asignacion</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>VARCHAR(200)</t>
+          <t>TIMESTAMP</t>
         </is>
       </c>
       <c r="D83" t="b">
@@ -2213,38 +2217,38 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notario_procurador_asociacion</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>estado_documento</t>
+          <t>fecha_reasignacion</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>VARCHAR(11)</t>
+          <t>TIMESTAMP</t>
         </is>
       </c>
       <c r="D84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notario_procurador_asociacion</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>notario_id</t>
+          <t>motivo_reasignacion</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(255)</t>
         </is>
       </c>
       <c r="D85" t="b">
@@ -2255,17 +2259,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notario_procurador_asociacion</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>procurador_id</t>
+          <t>activo</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D86" t="b">
@@ -2276,12 +2280,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notarios</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>bufete_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2290,61 +2294,61 @@
         </is>
       </c>
       <c r="D87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notarios</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>activo</t>
+          <t>numero_colegiado</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>VARCHAR(20)</t>
         </is>
       </c>
       <c r="D88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notarios</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>fecha_creacion</t>
+          <t>colegiado_activo</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>TIMESTAMP</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>documentos_notariales</t>
+          <t>notarios</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>fecha_actualizacion</t>
+          <t>fecha_verificacion</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2360,42 +2364,38 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>notario_asistente</t>
+          <t>notarios</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>firma_electronica_registrada</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="D91" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>nextval('notario_asistente_id_seq'::regclass)</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>notario_asistente</t>
+          <t>notarios</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>notario_id</t>
+          <t>proveedor_firma_electronica</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(100)</t>
         </is>
       </c>
       <c r="D92" t="b">
@@ -2406,12 +2406,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>notario_asistente</t>
+          <t>procuradores</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>asistente_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2420,14 +2420,14 @@
         </is>
       </c>
       <c r="D93" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>notario_procurador</t>
+          <t>documentos_notariales</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2445,51 +2445,722 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>nextval('notario_procurador_id_seq'::regclass)</t>
+          <t>nextval('documentos_notariales_id_seq'::regclass)</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>notario_procurador</t>
+          <t>documentos_notariales</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>notario_id</t>
+          <t>tipo_documento</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>INTEGER</t>
+          <t>VARCHAR(17)</t>
         </is>
       </c>
       <c r="D95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>numero_instrumento</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D96" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>fecha_otorgamiento</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="D97" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>hora_otorgamiento</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>TIME</t>
+        </is>
+      </c>
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>lugar_otorgamiento</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>VARCHAR(200)</t>
+        </is>
+      </c>
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>estado_documento</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>VARCHAR(11)</t>
+        </is>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>notario_id</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D101" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>procurador_id</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>bufete_id</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>BOOLEAN</t>
+        </is>
+      </c>
+      <c r="D104" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>fecha_creacion</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>TIMESTAMP</t>
+        </is>
+      </c>
+      <c r="D105" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>documentos_notariales</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>fecha_actualizacion</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>TIMESTAMP</t>
+        </is>
+      </c>
+      <c r="D106" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>notario_asistente</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>nextval('notario_asistente_id_seq'::regclass)</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>notario_asistente</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>notario_id</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D108" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>notario_asistente</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>asistente_id</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D109" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
           <t>notario_procurador</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>nextval('notario_procurador_id_seq'::regclass)</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>notario_procurador</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>notario_id</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>notario_procurador</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
         <is>
           <t>procurador_id</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>INTEGER</t>
-        </is>
-      </c>
-      <c r="D96" t="b">
-        <v>1</v>
-      </c>
-      <c r="E96" t="inlineStr"/>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D112" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>test_personas</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D113" t="b">
+        <v>0</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>nextval('test_personas_id_seq'::regclass)</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>test_personas</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>VARCHAR(120)</t>
+        </is>
+      </c>
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>test_personas</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>nit</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>VARCHAR(32)</t>
+        </is>
+      </c>
+      <c r="D115" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>test_personas</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>dpi</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>VARCHAR(32)</t>
+        </is>
+      </c>
+      <c r="D116" t="b">
+        <v>0</v>
+      </c>
+      <c r="E116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>test_personas</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>TIMESTAMP</t>
+        </is>
+      </c>
+      <c r="D117" t="b">
+        <v>0</v>
+      </c>
+      <c r="E117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>test_personas</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>nit_uq</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>VARCHAR(32)</t>
+        </is>
+      </c>
+      <c r="D118" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>geo_countries</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D119" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>nextval('geo_countries_id_seq'::regclass)</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>geo_countries</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>iso2</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>VARCHAR(2)</t>
+        </is>
+      </c>
+      <c r="D120" t="b">
+        <v>0</v>
+      </c>
+      <c r="E120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>geo_countries</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>iso3</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>VARCHAR(3)</t>
+        </is>
+      </c>
+      <c r="D121" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>geo_countries</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>VARCHAR(120)</t>
+        </is>
+      </c>
+      <c r="D122" t="b">
+        <v>0</v>
+      </c>
+      <c r="E122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>geo_admin1</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D123" t="b">
+        <v>0</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>nextval('geo_admin1_id_seq'::regclass)</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>geo_admin1</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>country_id</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>INTEGER</t>
+        </is>
+      </c>
+      <c r="D124" t="b">
+        <v>0</v>
+      </c>
+      <c r="E124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>geo_admin1</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>VARCHAR(10)</t>
+        </is>
+      </c>
+      <c r="D125" t="b">
+        <v>0</v>
+      </c>
+      <c r="E125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>geo_admin1</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>VARCHAR(120)</t>
+        </is>
+      </c>
+      <c r="D126" t="b">
+        <v>0</v>
+      </c>
+      <c r="E126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>geo_admin1</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>type_name</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>VARCHAR(40)</t>
+        </is>
+      </c>
+      <c r="D127" t="b">
+        <v>1</v>
+      </c>
+      <c r="E127" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>